<commit_message>
Entrega Final Laboratorio 7
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/2022-20/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\coding\EDA\Labs\lab_7\LabColisiones-L07-G08\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="726" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F54888-DFB5-49D6-8E23-12D138256747}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0834A9-0318-4926-BC48-4B8A684FF17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="887" windowWidth="2273" windowHeight="1493" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="2" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <r>
       <t>Factor de Carga</t>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Tiempo de Ejecución Real @SC [ms]</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -169,31 +172,25 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -205,14 +202,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -237,7 +240,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -366,6 +369,32 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -631,16 +660,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>25252.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>25235.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>25235.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>25235.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,16 +681,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>103.383</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>346.59199999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>247.185</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>257.38799999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,13 +791,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>25240.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>25235.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25235.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>25235.200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,13 +812,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>106.062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>118.133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122.46899999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>108.911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1346,16 +1381,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>25252.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>25235.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>25235.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>25235.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1504,13 +1539,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>25240.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>25235.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25235.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>25235.200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2890,7 +2928,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CAFD5B44-21B9-42C7-B503-C146EF1BA3EE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2901,7 +2939,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{680E7371-595A-4F03-ABE3-E0257A96E5F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2912,7 +2950,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2945,7 +2983,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2975,24 +3013,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
-    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:D14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A10:D14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E13AB410-EAE7-4700-B7BB-56834F33DA0E}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3295,27 +3334,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3326,119 +3365,120 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="10">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>0.1</v>
       </c>
       <c r="B3" s="5">
-        <v>100</v>
+        <v>25252.5</v>
       </c>
-      <c r="C3" s="8">
-        <v>75</v>
+      <c r="C3" s="7">
+        <v>103.383</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="11">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>0.5</v>
       </c>
-      <c r="B4" s="6">
-        <f>B3+40</f>
-        <v>140</v>
+      <c r="B4" s="2">
+        <v>25235.3</v>
       </c>
-      <c r="C4" s="8">
-        <f>C3+10</f>
-        <v>85</v>
+      <c r="C4" s="7">
+        <v>346.59199999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="10">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>0.7</v>
       </c>
-      <c r="B5" s="6">
-        <f>B4+40</f>
-        <v>180</v>
+      <c r="B5" s="2">
+        <v>25235.200000000001</v>
       </c>
-      <c r="C5" s="8">
-        <f>C4+10</f>
-        <v>95</v>
+      <c r="C5" s="7">
+        <v>247.185</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>0.9</v>
       </c>
-      <c r="B6" s="6">
-        <f>B5+40</f>
-        <v>220</v>
+      <c r="B6" s="2">
+        <v>25235.3</v>
       </c>
-      <c r="C6" s="8">
-        <f>C5+10</f>
-        <v>105</v>
+      <c r="C6" s="7">
+        <v>257.38799999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.5">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
     </row>
-    <row r="10" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" s="2">
-        <v>100</v>
+        <v>25240.6</v>
       </c>
       <c r="C11" s="5">
-        <v>105</v>
+        <v>106.062</v>
       </c>
+      <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2">
-        <f>B11+30</f>
-        <v>130</v>
+        <v>25235.200000000001</v>
       </c>
-      <c r="C12" s="6">
-        <f>C11+20</f>
-        <v>125</v>
+      <c r="C12" s="2">
+        <v>118.133</v>
       </c>
+      <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="2">
+        <v>25235.200000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>122.46899999999999</v>
+      </c>
+      <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>8</v>
       </c>
       <c r="B14" s="2">
-        <f>B12+30</f>
-        <v>160</v>
+        <v>25235.200000000001</v>
       </c>
-      <c r="C14" s="6">
-        <f>C12+20</f>
-        <v>145</v>
+      <c r="C14" s="2">
+        <v>108.911</v>
       </c>
+      <c r="D14" s="12"/>
     </row>
-    <row r="23" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="23" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -3453,6 +3493,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a4df9e4b793c0fa050084ef4feafa589">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="067b7080d2289f9ba15465beea7d18a8" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -3689,27 +3749,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF363B8-2236-4100-84F9-92CAF618B773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3726,29 +3791,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>